<commit_message>
added family promise census info
</commit_message>
<xml_diff>
--- a/exit destinations by percent.xlsx
+++ b/exit destinations by percent.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4556962025316456</v>
+        <v>0.3981900452488688</v>
       </c>
     </row>
     <row r="3">
@@ -390,17 +390,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.189873417721519</v>
+        <v>0.16289592760181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Rental by client with RRH or equivalent subsidy</t>
+          <t>No exit interview completed</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1265822784810127</v>
+        <v>0.09954751131221719</v>
       </c>
     </row>
     <row r="5">
@@ -410,17 +410,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0759493670886076</v>
+        <v>0.08144796380090498</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Transitional Housing for homeless persons (including homeless youth)</t>
+          <t>Rental by client with RRH or equivalent subsidy</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0759493670886076</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="7">
@@ -430,17 +430,77 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06329113924050633</v>
+        <v>0.04977375565610859</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>Staying or living with family, permanent tenure</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.04072398190045249</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Transitional Housing for homeless persons (including homeless youth)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.03619909502262444</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Hotel or Motel paid for without Emergency Shelter Voucher</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.01809954751131222</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Staying or living with family, temporary tenure (e.g., room, apartment or house)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.01357466063348416</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.009049773755656109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Substance Abuse Treatment or Detox Center</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.009049773755656109</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>Rental by client, other ongoing housing subsidy</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.01265822784810127</v>
+      <c r="B14" t="n">
+        <v>0.004524886877828055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>